<commit_message>
Percentages are now reported as decimals (ie. 98% = .98)
</commit_message>
<xml_diff>
--- a/IM-testing/[IM] Codebook2.xlsx
+++ b/IM-testing/[IM] Codebook2.xlsx
@@ -5349,6 +5349,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>68</xdr:row>
+      <xdr:rowOff>304800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 1" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5660,6 +5711,57 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 2" hidden="1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noSelect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="12700000" cy="12700000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -5929,10 +6031,10 @@
   <dimension ref="A1:Z1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C381" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A409" sqref="A409"/>
+      <selection pane="bottomRight" activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -6735,7 +6837,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="8" t="s">
+      <c r="A40" s="37" t="s">
         <v>111</v>
       </c>
       <c r="B40" s="13" t="s">
@@ -6775,7 +6877,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="8" t="s">
+      <c r="A42" s="37" t="s">
         <v>118</v>
       </c>
       <c r="B42" s="13" t="s">

</xml_diff>